<commit_message>
Added getCandidate and getLocations
</commit_message>
<xml_diff>
--- a/Elections2018.xlsx
+++ b/Elections2018.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idree\Documents\University\Year 2\Summer 2020\Object Oriented Software Design Analysis\Group Project\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1098A709-334B-459A-B82D-779FCB35C333}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1505C91C-64EB-4580-A164-9732DAA61A3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="4237" yWindow="1470" windowWidth="14400" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10546" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -1108,16 +1108,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F3058"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E3043" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A683" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="H184" sqref="H184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53125" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5.73046875" customWidth="1"/>
     <col min="2" max="2" width="4.59765625" customWidth="1"/>
-    <col min="3" max="3" width="59.796875" customWidth="1"/>
-    <col min="4" max="4" width="120.46484375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.06640625" customWidth="1"/>
+    <col min="4" max="4" width="17.3984375" customWidth="1"/>
     <col min="5" max="5" width="26.59765625" customWidth="1"/>
     <col min="6" max="6" width="5.46484375" customWidth="1"/>
   </cols>

</xml_diff>